<commit_message>
changed formulas from [] to {}
</commit_message>
<xml_diff>
--- a/output/output_name.xlsx
+++ b/output/output_name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,44 +439,73 @@
           <t>Formula1</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Formula2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>16</v>
       </c>
+      <c r="B2" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>14</v>
       </c>
+      <c r="B3" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>12</v>
       </c>
+      <c r="B4" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>10</v>
       </c>
+      <c r="B5" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>8</v>
       </c>
+      <c r="B6" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>4</v>
       </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>